<commit_message>
Add caching to improve app performance and fix net return display issues
</commit_message>
<xml_diff>
--- a/Aggregate Monthly RoA.xlsx
+++ b/Aggregate Monthly RoA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BW Code\CashDragProject\portfolio_optimizer_streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AA3827E-2799-4C07-B49C-7978C7CDBB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E1A288-E49C-403F-B435-8CCD17A99562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18015" yWindow="4665" windowWidth="27015" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32670" yWindow="120" windowWidth="24255" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Month</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>CLO AAA ETF F1</t>
+  </si>
+  <si>
+    <t>CLO MEZZ F1</t>
+  </si>
+  <si>
+    <t>TRUPS MEZZ F1</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -235,12 +241,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -251,6 +268,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,9 +577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AC22" sqref="AC22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -569,7 +592,7 @@
     <col min="26" max="26" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,8 +671,17 @@
       <c r="Z1" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -694,8 +726,9 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -740,8 +773,9 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -792,8 +826,9 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -844,8 +879,9 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -896,8 +932,9 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -948,8 +985,9 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1004,8 +1042,9 @@
         <v>2.0757035477932319E-2</v>
       </c>
       <c r="Z8" s="5"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -1062,8 +1101,9 @@
         <v>7.7303454332680764E-3</v>
       </c>
       <c r="Z9" s="5"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1128,8 +1168,9 @@
       <c r="Z10" s="5">
         <v>2.380923794495916E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA10" s="2"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -1196,8 +1237,9 @@
       <c r="Z11" s="5">
         <v>2.358809691728117E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1258,8 +1300,9 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1320,8 +1363,9 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1380,8 +1424,9 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1440,8 +1485,9 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA15" s="2"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1508,8 +1554,9 @@
       </c>
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -1576,8 +1623,9 @@
       </c>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1640,8 +1688,9 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA18" s="2"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
@@ -1704,8 +1753,9 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45778</v>
       </c>
@@ -1770,6 +1820,71 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
+      <c r="AA20" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45809</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="G21" s="6">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.84E-2</v>
+      </c>
+      <c r="J21" s="6">
+        <v>-5.1000000000000004E-3</v>
+      </c>
+      <c r="L21" s="6">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="M21" s="6">
+        <v>1.11E-2</v>
+      </c>
+      <c r="N21" s="6">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="P21" s="6">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>1.18E-2</v>
+      </c>
+      <c r="R21" s="6">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="S21" s="6">
+        <v>6.0100000000000001E-2</v>
+      </c>
+      <c r="T21" s="6">
+        <v>5.6500000000000002E-2</v>
+      </c>
+      <c r="U21" s="6">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="V21" s="6">
+        <v>1.09E-2</v>
+      </c>
+      <c r="W21" s="6">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="AB21" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AC21" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert smoothing changes to efficient frontier and remove 11.97% debugging code for better performance
</commit_message>
<xml_diff>
--- a/Aggregate Monthly RoA.xlsx
+++ b/Aggregate Monthly RoA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BW Code\CashDragProject\portfolio_optimizer_streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E1A288-E49C-403F-B435-8CCD17A99562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0B6E8-5991-49F7-919D-6EF826D2C7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32670" yWindow="120" windowWidth="24255" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3345" yWindow="1350" windowWidth="24255" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,14 +579,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AC22" sqref="AC22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
     <col min="24" max="24" width="15.42578125" customWidth="1"/>
     <col min="25" max="25" width="12.7109375" customWidth="1"/>
     <col min="26" max="26" width="14.5703125" customWidth="1"/>

</xml_diff>